<commit_message>
Edit etat paiement file format
</commit_message>
<xml_diff>
--- a/paiement.xlsx
+++ b/paiement.xlsx
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>28/08/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>nmaxies</t>
+          <t>Formation de relais</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>FRANCEGBE GHISLAINE NADIA</t>
+          <t>SEGLA MODESTE GBETOGNON</t>
         </is>
       </c>
       <c r="C8" s="6" t="n"/>
@@ -569,7 +569,7 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>MOUSSE FARDUKMARINO KAYOE</t>
+          <t>DEGUENON CINSOU JUDES CHARLES</t>
         </is>
       </c>
       <c r="C9" s="6" t="n"/>
@@ -583,7 +583,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>KPATCHAV ANOEL HIVERT</t>
+          <t>OUENSA GEO FROY MWILFRIED</t>
         </is>
       </c>
       <c r="C10" s="6" t="n"/>
@@ -597,7 +597,7 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>AHODEKON MAVIESNCAS VANDECEDAN</t>
+          <t>AGOI MARTIN</t>
         </is>
       </c>
       <c r="C11" s="6" t="n"/>
@@ -611,7 +611,7 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>ASSEKOUTOU MARTINE</t>
+          <t>AMOUSSOU PARFAIT</t>
         </is>
       </c>
       <c r="C12" s="6" t="n"/>
@@ -625,7 +625,7 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>ASSEKOUTOU MARTINE</t>
+          <t>ADEDE KOCOU ABRAHAM</t>
         </is>
       </c>
       <c r="C13" s="6" t="n"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>ASSEKOUTOU MARTINE</t>
+          <t>HOUNTONNAGNON CAKPO LUCIEN</t>
         </is>
       </c>
       <c r="C14" s="6" t="n"/>
@@ -653,7 +653,7 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>HOUNSOU LAHURNN MSLESSA</t>
+          <t>TCHOGNINOU MATHIAS</t>
         </is>
       </c>
       <c r="C15" s="6" t="n"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>HUNSOU LAHOUANNU BE LE SIA</t>
+          <t>ZINHOUEHOU DOROTHE</t>
         </is>
       </c>
       <c r="C16" s="6" t="n"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>HOUNSOU CARHUGNON REILE SIPHAN</t>
+          <t>FANOU SENOUMATE GEDEON</t>
         </is>
       </c>
       <c r="C17" s="6" t="n"/>
@@ -695,7 +695,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>HOUNSOU AHOUGNON ERCLLES ECHAIN</t>
+          <t>EKEHOUNDE ECUROSSE MICHELINE</t>
         </is>
       </c>
       <c r="C18" s="6" t="n"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>ASSOGBA JUNIAS ORTINEL</t>
+          <t>DAGBEGNON BONAVENTURE</t>
         </is>
       </c>
       <c r="C19" s="6" t="n"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>ASSOGBA JUNIAS ORTINEL</t>
+          <t>SOHOUNDJO MEREMIE DENANHOUEA</t>
         </is>
       </c>
       <c r="C20" s="6" t="n"/>
@@ -737,7 +737,7 @@
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>ALIGBONONSSI CLU AUUENUIENUIDOLONGBDAS</t>
+          <t>ADOKO LEA SONAGNON</t>
         </is>
       </c>
       <c r="C21" s="6" t="n"/>
@@ -751,7 +751,7 @@
       </c>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>ASLDU NOUNONVENAN FREDERIO</t>
+          <t>DOSSA ASYLVESTRE</t>
         </is>
       </c>
       <c r="C22" s="6" t="n"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>ABLOU NOUNONVENAN FREDERIC</t>
+          <t>TOBOSSI REFI</t>
         </is>
       </c>
       <c r="C23" s="6" t="n"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>ABLDU NOUNONVENAN FREDERIC</t>
+          <t>DOVONON CLEMENTINE</t>
         </is>
       </c>
       <c r="C24" s="6" t="n"/>
@@ -793,7 +793,7 @@
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>DANSOU ALIHONOU</t>
+          <t>GANSE SEWANOU ALBERTINE</t>
         </is>
       </c>
       <c r="C25" s="6" t="n"/>
@@ -807,7 +807,7 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>ADJVEHOUN BERNARD</t>
+          <t>KOUADOUA JULIETTE AYABA M</t>
         </is>
       </c>
       <c r="C26" s="6" t="n"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>ADJIVEHOUN BERNARD</t>
+          <t>LAWANI KADER</t>
         </is>
       </c>
       <c r="C27" s="6" t="n"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>ADJIVEHOUN BERNARD</t>
+          <t>AGNIZO VICTORINE</t>
         </is>
       </c>
       <c r="C28" s="6" t="n"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>EDAH CASIMIR</t>
+          <t>DOSSOUHOUI AHODEGNON ARMAND</t>
         </is>
       </c>
       <c r="C29" s="6" t="n"/>
@@ -863,7 +863,7 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>ATCHA WIL FRIED SEWACE</t>
+          <t>TCHOBO FAABO JANVIENNE</t>
         </is>
       </c>
       <c r="C30" s="6" t="n"/>
@@ -872,332 +872,38 @@
       <c r="F30" s="6" t="n"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="B31" s="5" t="inlineStr">
-        <is>
-          <t>ABLD NOANONVENAN FREDERIC</t>
-        </is>
-      </c>
-      <c r="C31" s="6" t="n"/>
+      <c r="A31" s="6" t="n"/>
+      <c r="B31" s="6" t="n"/>
+      <c r="C31" s="7" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
       <c r="D31" s="6" t="n"/>
       <c r="E31" s="6" t="n"/>
       <c r="F31" s="6" t="n"/>
     </row>
-    <row r="32" ht="15" customHeight="1">
-      <c r="A32" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="B32" s="5" t="inlineStr">
-        <is>
-          <t>ASSEKOUTOU MARTINE</t>
-        </is>
-      </c>
-      <c r="C32" s="6" t="n"/>
-      <c r="D32" s="6" t="n"/>
-      <c r="E32" s="6" t="n"/>
-      <c r="F32" s="6" t="n"/>
-    </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="B33" s="5" t="inlineStr">
-        <is>
-          <t>ASSEKOUTOU MARTINE</t>
-        </is>
-      </c>
-      <c r="C33" s="6" t="n"/>
-      <c r="D33" s="6" t="n"/>
-      <c r="E33" s="6" t="n"/>
-      <c r="F33" s="6" t="n"/>
-    </row>
-    <row r="34" ht="15" customHeight="1">
-      <c r="A34" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="B34" s="5" t="inlineStr">
-        <is>
-          <t>HOUNSOU CHOURN EL CAV</t>
-        </is>
-      </c>
-      <c r="C34" s="6" t="n"/>
-      <c r="D34" s="6" t="n"/>
-      <c r="E34" s="6" t="n"/>
-      <c r="F34" s="6" t="n"/>
-    </row>
-    <row r="35" ht="15" customHeight="1">
-      <c r="A35" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="B35" s="5" t="inlineStr">
-        <is>
-          <t>HOUNSOU MRELESCANE</t>
-        </is>
-      </c>
-      <c r="C35" s="6" t="n"/>
-      <c r="D35" s="6" t="n"/>
-      <c r="E35" s="6" t="n"/>
-      <c r="F35" s="6" t="n"/>
-    </row>
-    <row r="36" ht="15" customHeight="1">
-      <c r="A36" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="B36" s="5" t="inlineStr">
-        <is>
-          <t>ASSOGBA JUNIAS ORTINEL</t>
-        </is>
-      </c>
-      <c r="C36" s="6" t="n"/>
-      <c r="D36" s="6" t="n"/>
-      <c r="E36" s="6" t="n"/>
-      <c r="F36" s="6" t="n"/>
-    </row>
-    <row r="37" ht="15" customHeight="1">
-      <c r="A37" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="B37" s="5" t="inlineStr">
-        <is>
-          <t>ASSOGGA UNAS ORTINEL</t>
-        </is>
-      </c>
-      <c r="C37" s="6" t="n"/>
-      <c r="D37" s="6" t="n"/>
-      <c r="E37" s="6" t="n"/>
-      <c r="F37" s="6" t="n"/>
-    </row>
-    <row r="38" ht="15" customHeight="1">
-      <c r="A38" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="B38" s="5" t="inlineStr">
-        <is>
-          <t>ABLD NGNON.ENA FKEDERIC</t>
-        </is>
-      </c>
-      <c r="C38" s="6" t="n"/>
-      <c r="D38" s="6" t="n"/>
-      <c r="E38" s="6" t="n"/>
-      <c r="F38" s="6" t="n"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="B39" s="5" t="inlineStr">
-        <is>
-          <t>ABL OU NOUNONVENAN FREDERIC</t>
-        </is>
-      </c>
-      <c r="C39" s="6" t="n"/>
-      <c r="D39" s="6" t="n"/>
-      <c r="E39" s="6" t="n"/>
-      <c r="F39" s="6" t="n"/>
-    </row>
-    <row r="40" ht="15" customHeight="1">
-      <c r="A40" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="B40" s="5" t="inlineStr">
-        <is>
-          <t>ALIGBONONSS ODJONUUFHU CH OUDEO BIDIN</t>
-        </is>
-      </c>
-      <c r="C40" s="6" t="n"/>
-      <c r="D40" s="6" t="n"/>
-      <c r="E40" s="6" t="n"/>
-      <c r="F40" s="6" t="n"/>
-    </row>
-    <row r="41" ht="15" customHeight="1">
-      <c r="A41" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="B41" s="5" t="inlineStr">
-        <is>
-          <t>ALIGBONONSSI ODEIOUE LER BNTILON BDAS</t>
-        </is>
-      </c>
-      <c r="C41" s="6" t="n"/>
-      <c r="D41" s="6" t="n"/>
-      <c r="E41" s="6" t="n"/>
-      <c r="F41" s="6" t="n"/>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="B42" s="5" t="inlineStr">
-        <is>
-          <t>HOUEGLO BORIS DEODI</t>
-        </is>
-      </c>
-      <c r="C42" s="6" t="n"/>
-      <c r="D42" s="6" t="n"/>
-      <c r="E42" s="6" t="n"/>
-      <c r="F42" s="6" t="n"/>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="B43" s="5" t="inlineStr">
-        <is>
-          <t>KPEDOTOSSI FIFAME CARMELIA</t>
-        </is>
-      </c>
-      <c r="C43" s="6" t="n"/>
-      <c r="D43" s="6" t="n"/>
-      <c r="E43" s="6" t="n"/>
-      <c r="F43" s="6" t="n"/>
-    </row>
-    <row r="44" ht="15" customHeight="1">
-      <c r="A44" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="B44" s="5" t="inlineStr">
-        <is>
-          <t>KPATCHAVI NOEL HIVERTO</t>
-        </is>
-      </c>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-    </row>
-    <row r="45" ht="15" customHeight="1">
-      <c r="A45" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="B45" s="5" t="inlineStr">
-        <is>
-          <t>FRANCEGBE GHISLAINE NADNA</t>
-        </is>
-      </c>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-    </row>
-    <row r="46" ht="15" customHeight="1">
-      <c r="A46" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="B46" s="5" t="inlineStr">
-        <is>
-          <t>FRANCEGBE GHISLAINE NADIA</t>
-        </is>
-      </c>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-    </row>
-    <row r="47" ht="15" customHeight="1">
-      <c r="A47" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="B47" s="5" t="inlineStr">
-        <is>
-          <t>MOUSSE FARDUKMARINO KAYOE</t>
-        </is>
-      </c>
-      <c r="C47" s="6" t="n"/>
-      <c r="D47" s="6" t="n"/>
-      <c r="E47" s="6" t="n"/>
-      <c r="F47" s="6" t="n"/>
-    </row>
-    <row r="48" ht="15" customHeight="1">
-      <c r="A48" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="B48" s="5" t="inlineStr">
-        <is>
-          <t>AHOEKON MAMES NIAS VAN DE CEDAN</t>
-        </is>
-      </c>
-      <c r="C48" s="6" t="n"/>
-      <c r="D48" s="6" t="n"/>
-      <c r="E48" s="6" t="n"/>
-      <c r="F48" s="6" t="n"/>
-    </row>
-    <row r="49" ht="15" customHeight="1">
-      <c r="A49" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="B49" s="5" t="inlineStr">
-        <is>
-          <t>ADANMAZE LUCEN SOUROU GILDAS</t>
-        </is>
-      </c>
-      <c r="C49" s="6" t="n"/>
-      <c r="D49" s="6" t="n"/>
-      <c r="E49" s="6" t="n"/>
-      <c r="F49" s="6" t="n"/>
-    </row>
-    <row r="50" ht="15" customHeight="1">
-      <c r="A50" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="B50" s="5" t="inlineStr">
-        <is>
-          <t>MUSTINO ALINO</t>
-        </is>
-      </c>
-      <c r="C50" s="6" t="n"/>
-      <c r="D50" s="6" t="n"/>
-      <c r="E50" s="6" t="n"/>
-      <c r="F50" s="6" t="n"/>
-    </row>
-    <row r="51" ht="15" customHeight="1">
-      <c r="A51" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="B51" s="5" t="inlineStr">
-        <is>
-          <t>MUSTINC ALINO</t>
-        </is>
-      </c>
-      <c r="C51" s="6" t="n"/>
-      <c r="D51" s="6" t="n"/>
-      <c r="E51" s="6" t="n"/>
-      <c r="F51" s="6" t="n"/>
-    </row>
-    <row r="52" ht="15" customHeight="1">
-      <c r="A52" s="6" t="n"/>
-      <c r="B52" s="6" t="n"/>
-      <c r="C52" s="7" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="D52" s="6" t="n"/>
-      <c r="E52" s="6" t="n"/>
-      <c r="F52" s="6" t="n"/>
-    </row>
-    <row r="54">
-      <c r="B54" s="8" t="inlineStr">
+    <row r="33">
+      <c r="B33" s="8" t="inlineStr">
         <is>
           <t>Le Demandeur</t>
         </is>
       </c>
-      <c r="E54" s="8" t="inlineStr">
+      <c r="E33" s="8" t="inlineStr">
         <is>
           <t>Le Superviseur</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="B55" s="3" t="inlineStr">
-        <is>
-          <t>AHODEKON Maximes</t>
-        </is>
-      </c>
-      <c r="E55" s="3" t="inlineStr">
-        <is>
-          <t>nmaxies</t>
+    <row r="34">
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>AHODEKON Maxiès</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>.</t>
         </is>
       </c>
     </row>

</xml_diff>